<commit_message>
modified column names with color
</commit_message>
<xml_diff>
--- a/csv-excel/generated-file.xlsx
+++ b/csv-excel/generated-file.xlsx
@@ -25,12 +25,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -45,8 +50,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,94 +432,94 @@
           <t>s.no</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>EPIC ID</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>SPRINT ID</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>STORY ID</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>STORY DESCRIPTION</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>ASSIGNED TO</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>ESTIMATED
 STORY
 POINTS</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>STORY
 PLANNED
 START</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>STORY
 PLANNED
 END</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>ESTIMATED
 EFFORT
 (IN HRS))</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Time spent
 (IN Secs)</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>EFFORT
 CONSUMED
 (IN HRS)</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>PENDING
 EFFORT
 (IN HRS)</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>STORY
 ACTUAL
 START</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>STORY
 ACTUAL
 END</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>STORY
 Effort
@@ -521,21 +527,21 @@
 %</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">STORY
 Schedule
 Progress % </t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>STORY
 Schedule
 Overrun %</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
@@ -572,7 +578,6 @@
           <t>balachandras</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>20-05-2021</t>

</xml_diff>